<commit_message>
Add missing mandatory star.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Axiom_sample_preparation_v4_5_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Axiom_sample_preparation_v4_5_0.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="469">
   <si>
     <t xml:space="preserve">Axiom Sample Preparation Template</t>
   </si>
@@ -2082,7 +2082,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.4"/>
@@ -2092,7 +2092,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="31.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="35.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="36.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="36.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="37.49"/>
@@ -2243,7 +2243,9 @@
       <c r="M4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="N4" s="5"/>
+      <c r="N4" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="O4" s="2"/>
       <c r="P4" s="5" t="s">
         <v>3</v>
@@ -33402,7 +33404,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.49609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.43"/>

</xml_diff>